<commit_message>
Video Complete just needs writing on
</commit_message>
<xml_diff>
--- a/logbook.xlsx
+++ b/logbook.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Colorspaces" sheetId="1" r:id="rId1"/>
     <sheet name="Thresholding" sheetId="2" r:id="rId2"/>
+    <sheet name="Perspective" sheetId="4" r:id="rId3"/>
+    <sheet name="Gradient" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -194,6 +196,21 @@
   </si>
   <si>
     <t>V adds a few points through in the light shaded road which can only make it better</t>
+  </si>
+  <si>
+    <t>Kernal Size</t>
+  </si>
+  <si>
+    <t>Gradient</t>
+  </si>
+  <si>
+    <t>x 20 1000</t>
+  </si>
+  <si>
+    <t>Lines</t>
+  </si>
+  <si>
+    <t>Gets the outside edges of most lines. Lighter road gets the barrier rather than the road edge</t>
   </si>
 </sst>
 </file>
@@ -1372,6 +1389,55 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5467350" y="7143750"/>
+          <a:ext cx="4590001" cy="1440000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4590001</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>49350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="676275" y="381000"/>
           <a:ext cx="4590001" cy="1440000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1650,7 +1716,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
@@ -1875,11 +1941,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2015,4 +2081,110 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>620</v>
+      </c>
+      <c r="B1">
+        <v>425</v>
+      </c>
+      <c r="D1">
+        <v>650</v>
+      </c>
+      <c r="E1">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>170</v>
+      </c>
+      <c r="B2">
+        <v>720</v>
+      </c>
+      <c r="D2">
+        <v>1140</v>
+      </c>
+      <c r="E2">
+        <v>720</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="5">
+        <v>20100</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>